<commit_message>
Initial Schematic, Item list update
</commit_message>
<xml_diff>
--- a/ShowHerb-Item-List.xlsx
+++ b/ShowHerb-Item-List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marka\Downloads\Lab\new-project-template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marka\Downloads\Lab\ShowHerb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CEEF2A4-C9E0-4937-BBA1-58A4B8258E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9CA66F-3293-4B80-8E5F-A319E69C44A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accounting" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t xml:space="preserve">Item </t>
   </si>
@@ -55,6 +55,42 @@
   </si>
   <si>
     <t>Project Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arduino Nano 33 IoT </t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07VW9TSKD/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>Adafruit I2C Multiplexer</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B017C09ETS/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STEMMA Soil Sensor </t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/4026?gclid=Cj0KCQjwl_SHBhCQARIsAFIFRVXqnetQca0YiH1L4WKDv7rMAurkYQ8s318Mtg1VIUXXEpn5wohOilwaAkpSEALw_wcB</t>
+  </si>
+  <si>
+    <t>12V 1/2'' Electric Solenoid Valve</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07NWCRM75/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5V Relay </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elegoo Kit </t>
   </si>
 </sst>
 </file>
@@ -443,7 +479,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,40 +518,106 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E2" s="4"/>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>15</v>
+      </c>
       <c r="F2" s="4">
         <f>D2*E2</f>
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="I2" s="9">
         <f>SUM(F2:F50)</f>
-        <v>0</v>
+        <v>66.5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E3" s="4"/>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>8.5</v>
+      </c>
       <c r="F3" s="4">
         <f t="shared" ref="F3:F66" si="0">D3*E3</f>
-        <v>0</v>
+        <v>8.5</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E4" s="4"/>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>7.5</v>
+      </c>
       <c r="F4" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E5" s="4"/>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>13</v>
+      </c>
       <c r="F5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E6" s="4"/>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
       <c r="F6" s="4">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
Added to item list, added multiple 3D models, update main testing code.
</commit_message>
<xml_diff>
--- a/ShowHerb-Item-List.xlsx
+++ b/ShowHerb-Item-List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marka\Downloads\Lab\ShowHerb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9CA66F-3293-4B80-8E5F-A319E69C44A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F394F161-30FA-4C03-BD59-AA4817A55C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accounting" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t xml:space="preserve">Item </t>
   </si>
@@ -57,15 +57,9 @@
     <t>Project Total</t>
   </si>
   <si>
-    <t xml:space="preserve">Arduino Nano 33 IoT </t>
-  </si>
-  <si>
     <t>Amazon</t>
   </si>
   <si>
-    <t>https://www.amazon.com/gp/product/B07VW9TSKD/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;psc=1</t>
-  </si>
-  <si>
     <t>Adafruit I2C Multiplexer</t>
   </si>
   <si>
@@ -91,6 +85,48 @@
   </si>
   <si>
     <t xml:space="preserve">Elegoo Kit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arduino Nano Every </t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07YQ56B6Q/ref=ppx_yo_dt_b_asin_title_o04_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBSS Solderable Breadboard Pack </t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B082PX1GKT/ref=ppx_yo_dt_b_asin_title_o03_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glarks M3-M5 Female Threaded/Knurled Inserts </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon </t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07L96KVP3/ref=ppx_yo_dt_b_asin_title_o02_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>Virgue M3-M5 Hex Socket Button Cap Screws</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07HVRJW5J/ref=ppx_od_dt_b_asin_title_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>Photoresistor</t>
+  </si>
+  <si>
+    <t>Teyleten Rain Sensor</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B088FXM2JG/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>Hatchbox PLA</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B00J0ECR5I/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1</t>
   </si>
 </sst>
 </file>
@@ -479,13 +515,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="3"/>
-    <col min="2" max="3" width="26.77734375" customWidth="1"/>
+    <col min="2" max="2" width="38.21875" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="9"/>
     <col min="6" max="6" width="17.6640625" style="9" customWidth="1"/>
@@ -517,37 +554,37 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F2" s="4">
         <f>D2*E2</f>
         <v>30</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>9</v>
+      <c r="G2" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="I2" s="9">
         <f>SUM(F2:F50)</f>
-        <v>66.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>135.19999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -559,16 +596,16 @@
         <f t="shared" ref="F3:F66" si="0">D3*E3</f>
         <v>8.5</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -580,16 +617,16 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>14</v>
+      <c r="G4" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -602,15 +639,15 @@
         <v>13</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -623,41 +660,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E7" s="4"/>
+    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>21.7</v>
+      </c>
       <c r="F7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>21.7</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9">
+        <v>18</v>
+      </c>
       <c r="F8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>23</v>
+      </c>
       <c r="F9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
       <c r="F10" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" s="9">
+        <v>2</v>
+      </c>
       <c r="F11" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
       <c r="F12" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1189,7 +1309,17 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{D3242D99-B84E-406E-9AB5-A0057A363509}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{76B80C52-4BA4-4867-9A52-9EA24FA27F1D}"/>
+    <hyperlink ref="G7" r:id="rId3" xr:uid="{143F6426-4066-40ED-AC38-09D2D6EFAF45}"/>
+    <hyperlink ref="G8" r:id="rId4" xr:uid="{3F65B5E8-8BBA-4514-B9A2-60CF3EEA7B6F}"/>
+    <hyperlink ref="G9" r:id="rId5" xr:uid="{C108AAAC-BFFA-4878-BFEA-F264DA85383D}"/>
+    <hyperlink ref="G11" r:id="rId6" xr:uid="{35572192-A9DB-4111-94FA-69DA288151A0}"/>
+    <hyperlink ref="G12" r:id="rId7" xr:uid="{F098A064-06F5-4675-BE81-7A4FBA513BD1}"/>
+    <hyperlink ref="G4" r:id="rId8" xr:uid="{262815F4-5062-4268-867B-E31C581D33CB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>